<commit_message>
Fix Tracker.sq:add not returning id
</commit_message>
<xml_diff>
--- a/src/test/resources/members.xlsx
+++ b/src/test/resources/members.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ithersta/preaccelerator-bot/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9622E79B-BD6C-7D43-BCE7-B8157FE5366E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119E2560-4597-2B45-BF46-8A4B81279B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27660" yWindow="600" windowWidth="23420" windowHeight="28080" activeTab="1" xr2:uid="{99E25726-31D8-AF44-AC03-06A3F944462F}"/>
+    <workbookView xWindow="12560" yWindow="14700" windowWidth="24340" windowHeight="13980" activeTab="1" xr2:uid="{99E25726-31D8-AF44-AC03-06A3F944462F}"/>
   </bookViews>
   <sheets>
     <sheet name="Участники" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Номер телефона</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>+79000000011</t>
+  </si>
+  <si>
+    <t>Номер телефона трекера</t>
   </si>
 </sst>
 </file>
@@ -102,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -481,25 +485,25 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">

</xml_diff>